<commit_message>
bases clean (scss, plus de JS)
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -41,6 +41,15 @@
   </si>
   <si>
     <t xml:space="preserve">(SEO ou accessiblité ?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prevention prevenir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action guerir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">performance et vitesse</t>
   </si>
 </sst>
 </file>
@@ -249,13 +258,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z16"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.29"/>
@@ -310,9 +319,17 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>9</v>
+      </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
CSS terminé V.2 (avant mots clés)
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">Référence</t>
   </si>
   <si>
+    <t xml:space="preserve">meta téléphone réécrit</t>
+  </si>
+  <si>
     <t xml:space="preserve">(SEO ou accessiblité ?)</t>
   </si>
   <si>
@@ -49,17 +52,111 @@
     <t xml:space="preserve">action guerir</t>
   </si>
   <si>
+    <t xml:space="preserve">ajout du titre du site</t>
+  </si>
+  <si>
     <t xml:space="preserve">performance et vitesse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajout de &lt;script&gt; font awesome &lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accessibilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responsive mal construit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visibilité et accessibilité de certains éléments mauvaise </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bien intégrer la balise méta &lt;meta name="viewport" content="width=device-width"&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">commencer l’intégration du site en mobile first puis gérer le responsive tablette, desktop et grands ecrans en fonction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changement du nom de la page deux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom/titre du site manquant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pas de nom de site écrit en haut de la page, mauvais pour l’indexation etc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intégrer le titre entre les balises &lt;title&gt;&lt;/title&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle navigation enlevé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO/accessibilité/performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balise script pour font awesome non intégrée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pas d’accès aux icones voulues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intégrer le code entre balise &lt;script&gt; donné par font awesome, pour faire en sorte que les icones soient affichées et affichables sur le site par tous les navigateurs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bonnes balises utilisées (header, footer, div, nav, etc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEO/accessibilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page 2 sans réel nom </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pas de title explicite de la « page 2 », on ne sait pas ce que c’est au premier abord, encore moins Google qui ne saura pas de quoi parle cette page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">titres écrit et pas en photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggle navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alt des images faits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meilleure lisibilité du texte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fichier css mis dans le bon dossier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fichier scss fait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS supprimé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHANGER LES MOT CLES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compression des images ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parametrez le cache navigateur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -91,6 +188,20 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -107,12 +218,11 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,13 +235,32 @@
         <bgColor rgb="FF993366"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -160,7 +289,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -173,11 +302,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -236,7 +393,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
@@ -260,19 +417,21 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.32421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.34765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="55.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="121.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="69.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="96.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="44.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="10.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -294,95 +453,310 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="G1" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
+      <c r="A2" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4" t="s">
         <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="G3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="G5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="G6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="G7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="E8" s="2"/>
+      <c r="G8" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C9" s="11"/>
+      <c r="E9" s="2"/>
+      <c r="G9" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E9" s="4"/>
+      <c r="H9" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E10" s="4"/>
+      <c r="E10" s="2"/>
+      <c r="G10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E12" s="4"/>
+      <c r="E11" s="2"/>
+      <c r="G11" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E12" s="2"/>
+      <c r="G12" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E13" s="4"/>
+      <c r="E13" s="2"/>
+      <c r="G13" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E14" s="4"/>
+      <c r="E14" s="2"/>
+      <c r="G14" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="E15" s="2"/>
+      <c r="G15" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G16" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G17" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G18" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G19" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G20" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G21" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G22" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G23" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G24" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G25" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G26" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G27" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G28" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G29" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G30" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="H30" s="6"/>
+    </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1354,6 +1728,10 @@
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Ajout de meta description
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -53,8 +53,8 @@
   </si>
   <si>
     <t xml:space="preserve">bien intégrer la balise &lt;meta name="viewport" content="width=device-width"&gt;. 
-Commencer l’intégration  du site en mobile first pour plus facilement gérer le 
-Responsive tablette, desktop et grands ecrans ensuite</t>
+Commencer l’intégration du site en mobile first pour plus facilement gérer le 
+Responsive tablette, desktop et grands ecrans ensuite.</t>
   </si>
   <si>
     <t xml:space="preserve">Refaire l’intégration du style en mobile first.</t>
@@ -96,8 +96,7 @@
 La concernant sur les autres pages.</t>
   </si>
   <si>
-    <t xml:space="preserve">Accessibilité et SEO 
-Et Performance</t>
+    <t xml:space="preserve">Accessibilité et SEO et Performance</t>
   </si>
   <si>
     <t xml:space="preserve">« Toggle navigation » inutile</t>
@@ -106,7 +105,7 @@
     <t xml:space="preserve">Bloc inutile présent qui prend de la place dans le code et alourdit la page pour rien.</t>
   </si>
   <si>
-    <t xml:space="preserve">Faire une pré-maquette pour savori comment bien structurer le futur code.</t>
+    <t xml:space="preserve">Faire une pré-maquette pour savoir comment bien structurer le futur code.</t>
   </si>
   <si>
     <t xml:space="preserve">Bien suivre le web design et le suivre petit à petit pour ne rien louper ou ne rien ajouter de trop.</t>
@@ -248,11 +247,11 @@
   <si>
     <t xml:space="preserve">Ecrire les bons noms d’images permet de plus rapidement les identifier pour nous
 et pour les robots de mieux savoir de quoi elles « parlent » et de pouvoir s’appuyer
-Dessus en cas de requetes d’images. Sans espaces, sans caractères spéciaux et 
-Sans caractères accentués. Intégrer les </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Réécrire tous les noms des images, et les réintégrer en écrivant le bon chemin de pages.</t>
+dessus en cas de requetes d’images. Sans espaces, sans caractères spéciaux et 
+Sans caractères accentués.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réécrire tous les noms des images, et les réintégrer en écrivant le bon chemin d’accès.</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.nosyweb.fr/optimiser-mon-referencement-seo-joomla/comment-nommer-les-images-pour-un-site-internet.html</t>
@@ -265,7 +264,7 @@
   </si>
   <si>
     <t xml:space="preserve">mettre une taille de police de minimum 10px et préférer les unités comme le em ou 
-Le rem plutot que les unités fixes comme le px</t>
+Le rem plutot que les unités fixes comme le px.</t>
   </si>
   <si>
     <t xml:space="preserve">Changer tous les textes inférieur à 10px pour les intégrer à minimum 10px, et utiliser une unité comme le em ou le 
@@ -428,7 +427,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -439,6 +438,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF993366"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -476,7 +481,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -523,6 +528,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -612,8 +621,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D8" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E44" activeCellId="0" sqref="E44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -735,7 +744,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
         <v>23</v>
       </c>
@@ -782,7 +791,7 @@
       <c r="B13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="12" t="s">
         <v>36</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -855,14 +864,14 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" s="12" customFormat="true" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
+    <row r="21" s="13" customFormat="true" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="13" t="s">
         <v>55</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -1942,7 +1951,7 @@
       <c r="D25" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="14" t="s">
         <v>67</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -1962,7 +1971,7 @@
       <c r="D27" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="14" t="s">
         <v>73</v>
       </c>
       <c r="F27" s="1" t="s">

</xml_diff>

<commit_message>
ajout d'une classe au logo du header de la page contact
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -139,10 +139,10 @@
     <t xml:space="preserve">Meta description vide</t>
   </si>
   <si>
-    <t xml:space="preserve">Savoir si on ajoute ou non une meta description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si on a une meta descritpion, l’intégrer, sinon on ne met pas de meta description du tout.</t>
+    <t xml:space="preserve">Créer une meta description.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intégrer la meta description.</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.alsacreations.com/article/lire/628-balises-meta.html#utilite</t>
@@ -267,14 +267,29 @@
 Le rem plutot que les unités fixes comme le px.</t>
   </si>
   <si>
-    <t xml:space="preserve">Changer tous les textes inférieur à 10px pour les intégrer à minimum 10px, et utiliser une unité comme le em ou le 
-Rem.</t>
+    <t xml:space="preserve">Changer tous les textes inférieur à 10px pour les intégrer à minimum 10px, et utiliser une unité relative comme le em ou le Rem.</t>
   </si>
   <si>
     <t xml:space="preserve">http://all-for-design.com/web-design/lisibilite-des-sites-web-font-size-100-16px/</t>
   </si>
   <si>
     <t xml:space="preserve">Performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas de dossier ni fichier Sass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas de dossier ni fichier scss.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’utilisation de fichiers scss permet de compiler les fichiers css reliés aux pages. 
+Cela améliore la vitesse de chargement des pages.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer des fichiers scss dans un dossier scss.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://ipssidm.com/raisons-dabandonner-css-classique-sass/</t>
   </si>
   <si>
     <t xml:space="preserve">Fichier CSS « rangé » au mauvais endroit</t>
@@ -293,22 +308,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.ornitorinc.com/blog/referencement/10-bonnes-pratiques-referencement-seo/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pas de dossier ni fichier Sass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pas de dossier ni fichier scss.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’utilisation de fichiers scss permet de compiler les fichiers css reliés aux pages. 
-Cela améliore la vitesse de chargement des pages.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Créer des fichiers scss dans un dossier scss.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ipssidm.com/raisons-dabandonner-css-classique-sass/</t>
   </si>
   <si>
     <t xml:space="preserve">Javascript inutile</t>
@@ -427,7 +426,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -438,12 +437,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF993366"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -530,7 +523,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -621,8 +614,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -636,7 +629,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="9.61"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -674,13 +667,13 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="46.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -700,11 +693,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="46.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>13</v>
       </c>
@@ -724,7 +717,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="32.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
@@ -744,7 +738,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="32.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
         <v>23</v>
       </c>
@@ -764,7 +759,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="32.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -784,7 +780,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
@@ -804,7 +801,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="32.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
@@ -824,7 +822,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
         <v>13</v>
       </c>
@@ -844,7 +843,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="32.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -864,7 +864,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" s="13" customFormat="true" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" s="13" customFormat="true" ht="46.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
         <v>13</v>
       </c>
@@ -884,7 +885,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0"/>
       <c r="B22" s="0"/>
       <c r="C22" s="0"/>
@@ -1910,7 +1911,7 @@
       <c r="AMI22" s="0"/>
       <c r="AMJ22" s="0"/>
     </row>
-    <row r="23" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="74" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
@@ -1930,7 +1931,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
       <c r="B24" s="0"/>
       <c r="C24" s="0"/>
@@ -1938,7 +1939,7 @@
       <c r="E24" s="0"/>
       <c r="F24" s="0"/>
     </row>
-    <row r="25" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="46.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>7</v>
       </c>
@@ -1958,11 +1959,19 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0"/>
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+      <c r="D26" s="0"/>
+      <c r="E26" s="0"/>
+      <c r="F26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="32.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="12" t="s">
         <v>70</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1971,18 +1980,19 @@
       <c r="D27" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="5" t="s">
         <v>73</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="46.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="12" t="s">
         <v>75</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1991,14 +2001,15 @@
       <c r="D29" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="14" t="s">
         <v>78</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="18.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>69</v>
       </c>
@@ -2018,7 +2029,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="46.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>69</v>
       </c>
@@ -2038,10 +2050,10 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E34" s="5"/>
     </row>
-    <row r="35" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="32.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>69</v>
       </c>

</xml_diff>